<commit_message>
Update for end of 2023-2024
</commit_message>
<xml_diff>
--- a/docs/3369975a9851e6fd41a0ae6865456662040af596/Project_Info/Progress.xlsx
+++ b/docs/3369975a9851e6fd41a0ae6865456662040af596/Project_Info/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\csrf_hh_data\Project Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52E102-FC84-4C0E-A762-BE1AAC958015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56BC9C8-88C2-4504-A985-807FAFF5AC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4146" yWindow="3774" windowWidth="15360" windowHeight="9156" xr2:uid="{CCDAA5C6-C418-46A5-B53C-B8EF22BA8FD6}"/>
+    <workbookView xWindow="3504" yWindow="3204" windowWidth="18228" windowHeight="10818" activeTab="2" xr2:uid="{CCDAA5C6-C418-46A5-B53C-B8EF22BA8FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Geoduck" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Manila_Clam" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>#</t>
   </si>
@@ -58,18 +57,6 @@
     <t>Standardized catch per unit effort</t>
   </si>
   <si>
-    <t>bla1</t>
-  </si>
-  <si>
-    <t>bla2</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Selectivity parameterized by age </t>
   </si>
   <si>
@@ -104,6 +91,90 @@
   </si>
   <si>
     <t xml:space="preserve">Dr M. Mazur (DFO) developed a generalized linear model to standardize commercial catch data according to various variates. The model included temporal autocorrelation to prevent the estimation of large, implausible differences in inferred abundance. </t>
+  </si>
+  <si>
+    <t>Goes to 2022</t>
+  </si>
+  <si>
+    <t>Includes IFMP survey data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age composition data </t>
+  </si>
+  <si>
+    <t>All data sources updated to 2022</t>
+  </si>
+  <si>
+    <t>Most recent data points were included which allow for use of the index in simulated projections (as a basis for responsive management)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From annulus data, now included and assumed to be linked to the survey index series. </t>
+  </si>
+  <si>
+    <t>Placeholder for fishery effort data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model can be configured to include a metric of exploitation rate based on slip data (effort days). </t>
+  </si>
+  <si>
+    <t>Revised to subarea models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spatial unit changed back to subarea to allow for complete catch, density and biomass reporting for each model. </t>
+  </si>
+  <si>
+    <t>Top 10 by landings</t>
+  </si>
+  <si>
+    <t>Ten operating models were configured based on the ten subareas with the most contributory historical landings</t>
+  </si>
+  <si>
+    <t>Density included for MPs</t>
+  </si>
+  <si>
+    <t>By including observations of survey density it is now possible to configure management procedures and opening/closing rules based on simulated density observations</t>
+  </si>
+  <si>
+    <t>Models updated to include catch history</t>
+  </si>
+  <si>
+    <t>Catches incorporated to inform model scale</t>
+  </si>
+  <si>
+    <t>Model includes  nominal CPUE</t>
+  </si>
+  <si>
+    <t>This is a placeholder for standardized CPUE in a revision of the models</t>
+  </si>
+  <si>
+    <t>Multispecies survey density included</t>
+  </si>
+  <si>
+    <t>To allow for the testing of density-based management procedures linked to simulated density</t>
+  </si>
+  <si>
+    <t>Survey relative biomass in legal / sublegal size classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two additional indices included that are for legal and sublegal size classes providing information about the population structure and potentially allowing for management procedures that can account for shifts in size composition. </t>
+  </si>
+  <si>
+    <t>Size composition data included for both fleet and survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two sources of size composition data were combined in model conditioning for Stat. areas 12 and 19 that are relatively 'data rich' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development of responsive management procedures </t>
+  </si>
+  <si>
+    <t>Allows for the testing of adaptable harvest rate policies and open/closure rules</t>
+  </si>
+  <si>
+    <t>Rotational closure management procedures</t>
+  </si>
+  <si>
+    <t>Allows for evaluation of risk equivalency among harvest rates with and without rotational closures</t>
   </si>
 </sst>
 </file>
@@ -147,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -158,8 +229,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C6CC2D-3873-40C7-ACC0-7E4C4205C2EE}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -506,7 +583,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -539,7 +616,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -547,10 +624,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -558,10 +635,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -569,10 +646,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -580,10 +657,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -591,10 +668,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -604,10 +681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A8E84B-D3D7-4F95-A336-48FC4D6B0FC9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -632,10 +709,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -643,10 +720,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -656,10 +766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9844F237-2161-4893-A1F2-32AE6084B95F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -684,10 +794,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -695,10 +805,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -708,21 +851,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE2A605-E701-4B68-B98E-EAF5B3F977AB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" style="4"/>
+    <col min="1" max="1" width="8.83984375" style="6"/>
     <col min="2" max="2" width="26.15625" style="2" customWidth="1"/>
     <col min="3" max="3" width="121.5234375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -733,25 +876,44 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>